<commit_message>
get insight of QT signal and slot
</commit_message>
<xml_diff>
--- a/doc/驱动器通讯协议.xlsx
+++ b/doc/驱动器通讯协议.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -134,10 +134,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>通讯速度:9600 bp(RS485)s,  250K bps(CAN)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>校验计算暂时空</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -230,10 +226,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>判断类型: 1-"&gt;"; 2-"="; 3-"&lt;";   结果: 条件满足:1, 条件不满足</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>0x01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -267,14 +259,22 @@
   </si>
   <si>
     <t>电流档位:1-32</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通讯速度:9600 bp(RS485)s,  250K bps(CAN) 数据长度为8个字节</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>判断类型: 1-"&gt;"; 2-"="; 3-"&lt;";   结果: 条件满足:1, 条件不满足:0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -362,7 +362,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -371,15 +371,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -426,7 +462,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,9 +494,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,6 +529,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -667,14 +705,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L45" sqref="L45"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="5" width="9" style="1"/>
     <col min="6" max="6" width="13" style="1" bestFit="1" customWidth="1"/>
@@ -683,25 +721,25 @@
     <col min="12" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A1" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-    </row>
-    <row r="2" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A2" s="8" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="11" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8"/>
+      <c r="B2" s="11"/>
       <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
@@ -727,14 +765,14 @@
         <v>16</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A3" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
@@ -760,8 +798,8 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="5" spans="1:12" s="2" customFormat="1" ht="23.25" customHeight="1">
+    <row r="4" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="5" spans="1:12" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="9" t="s">
         <v>0</v>
       </c>
@@ -770,30 +808,30 @@
         <v>20</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E5" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G5" s="9"/>
       <c r="H5" s="9"/>
       <c r="I5" s="9"/>
       <c r="J5" s="5"/>
       <c r="K5" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="9"/>
       <c r="B6" s="9"/>
       <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>26</v>
@@ -812,11 +850,11 @@
       </c>
       <c r="J6" s="5"/>
       <c r="K6" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="8" spans="1:12" s="2" customFormat="1" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="8" spans="1:12" s="2" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="9" t="s">
         <v>0</v>
       </c>
@@ -825,30 +863,30 @@
         <v>21</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E8" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G8" s="9"/>
       <c r="H8" s="9"/>
       <c r="I8" s="9"/>
       <c r="J8" s="5"/>
       <c r="K8" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="9"/>
       <c r="B9" s="9"/>
       <c r="C9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>26</v>
@@ -867,11 +905,11 @@
       </c>
       <c r="J9" s="5"/>
       <c r="K9" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="11" spans="1:12" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="11" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="9" t="s">
         <v>0</v>
       </c>
@@ -880,30 +918,30 @@
         <v>19</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E11" s="5" t="s">
         <v>26</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="9"/>
       <c r="J11" s="5"/>
       <c r="K11" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E12" s="5" t="s">
         <v>26</v>
@@ -922,31 +960,31 @@
       </c>
       <c r="J12" s="5"/>
       <c r="K12" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A13" s="8"/>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A14" s="8"/>
-      <c r="B14" s="8"/>
-    </row>
-    <row r="15" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="11"/>
+      <c r="B13" s="11"/>
+    </row>
+    <row r="14" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+    </row>
+    <row r="15" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>26</v>
@@ -959,51 +997,51 @@
       </c>
       <c r="J15" s="5"/>
       <c r="K15" s="5" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="9"/>
       <c r="B16" s="9"/>
       <c r="C16" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>38</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>39</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G16" s="9"/>
       <c r="H16" s="9"/>
       <c r="I16" s="9"/>
       <c r="J16" s="5"/>
       <c r="K16" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
-      <c r="C17" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-    </row>
-    <row r="18" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C17" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="11"/>
+    </row>
+    <row r="18" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+    <row r="19" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+    <row r="20" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="9" t="s">
         <v>0</v>
       </c>
@@ -1012,36 +1050,36 @@
         <v>23</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G20" s="9"/>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
       <c r="J20" s="6"/>
       <c r="K20" s="6" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="9"/>
       <c r="B21" s="9"/>
       <c r="C21" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>26</v>
@@ -1054,12 +1092,12 @@
       </c>
       <c r="J21" s="6"/>
       <c r="K21" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="C22" s="10" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
       <c r="D22" s="10"/>
       <c r="E22" s="10"/>
@@ -1070,46 +1108,46 @@
       <c r="J22" s="10"/>
       <c r="K22" s="10"/>
     </row>
-    <row r="23" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
+    <row r="23" spans="1:12" s="3" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="11"/>
+      <c r="B23" s="11"/>
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:12" ht="23.25" customHeight="1">
+    <row r="24" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D24" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="9" t="s">
         <v>54</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="9" t="s">
-        <v>56</v>
       </c>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
       <c r="I24" s="9"/>
       <c r="J24" s="6"/>
       <c r="K24" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L24" s="3"/>
     </row>
-    <row r="25" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
+    <row r="25" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="9"/>
       <c r="B25" s="9"/>
       <c r="C25" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>26</v>
@@ -1128,17 +1166,17 @@
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="27" spans="1:12" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>17</v>
@@ -1147,22 +1185,22 @@
         <v>26</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
       <c r="J27" s="6"/>
       <c r="K27" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
+    <row r="28" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="9"/>
       <c r="B28" s="9"/>
       <c r="C28" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>18</v>
@@ -1184,17 +1222,17 @@
       </c>
       <c r="J28" s="6"/>
       <c r="K28" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="30" spans="1:12" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>17</v>
@@ -1203,22 +1241,22 @@
         <v>26</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G30" s="9"/>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="6"/>
       <c r="K30" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L30" s="3"/>
     </row>
-    <row r="31" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
+    <row r="31" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="9"/>
       <c r="B31" s="9"/>
       <c r="C31" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>18</v>
@@ -1240,20 +1278,20 @@
       </c>
       <c r="J31" s="6"/>
       <c r="K31" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="8"/>
-    </row>
-    <row r="33" spans="1:12" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="11"/>
+      <c r="B32" s="11"/>
+    </row>
+    <row r="33" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>17</v>
@@ -1269,15 +1307,15 @@
       <c r="I33" s="9"/>
       <c r="J33" s="6"/>
       <c r="K33" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
+    <row r="34" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="9"/>
       <c r="B34" s="9"/>
       <c r="C34" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>18</v>
@@ -1299,14 +1337,14 @@
       </c>
       <c r="J34" s="6"/>
       <c r="K34" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="8"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="10" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D35" s="10"/>
       <c r="E35" s="10"/>
@@ -1315,16 +1353,16 @@
       <c r="H35" s="10"/>
       <c r="I35" s="10"/>
       <c r="J35" s="10"/>
-      <c r="K35" s="11"/>
-    </row>
-    <row r="36" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="37" spans="1:12" ht="23.25" customHeight="1">
+      <c r="K35" s="8"/>
+    </row>
+    <row r="36" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>17</v>
@@ -1338,15 +1376,15 @@
       <c r="I37" s="9"/>
       <c r="J37" s="6"/>
       <c r="K37" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
+    <row r="38" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="9"/>
       <c r="B38" s="9"/>
       <c r="C38" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>18</v>
@@ -1368,14 +1406,14 @@
       </c>
       <c r="J38" s="6"/>
       <c r="K38" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
-      <c r="A39" s="11"/>
-      <c r="B39" s="11"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="8"/>
+      <c r="B39" s="8"/>
       <c r="C39" s="10" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D39" s="10"/>
       <c r="E39" s="10"/>
@@ -1383,17 +1421,17 @@
       <c r="G39" s="10"/>
       <c r="H39" s="10"/>
       <c r="I39" s="10"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-    </row>
-    <row r="40" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="41" spans="1:12" ht="23.25" customHeight="1">
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>17</v>
@@ -1407,15 +1445,15 @@
       <c r="I41" s="9"/>
       <c r="J41" s="6"/>
       <c r="K41" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
+    <row r="42" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="9"/>
       <c r="B42" s="9"/>
       <c r="C42" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>18</v>
@@ -1437,28 +1475,28 @@
       </c>
       <c r="J42" s="6"/>
       <c r="K42" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1">
-      <c r="C43" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-      <c r="F43" s="8"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="8"/>
-      <c r="I43" s="8"/>
-    </row>
-    <row r="44" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1"/>
-    <row r="45" spans="1:12" ht="23.25" customHeight="1">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="C43" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D43" s="11"/>
+      <c r="E43" s="11"/>
+      <c r="F43" s="11"/>
+      <c r="G43" s="11"/>
+      <c r="H43" s="11"/>
+      <c r="I43" s="11"/>
+    </row>
+    <row r="44" spans="1:12" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="9" t="s">
         <v>0</v>
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>17</v>
@@ -1472,15 +1510,15 @@
       <c r="I45" s="9"/>
       <c r="J45" s="6"/>
       <c r="K45" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="1:12" ht="23.25" customHeight="1">
+    <row r="46" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="9"/>
       <c r="B46" s="9"/>
       <c r="C46" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>18</v>
@@ -1502,77 +1540,67 @@
       </c>
       <c r="J46" s="6"/>
       <c r="K46" s="6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-      <c r="F47" s="8"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="8"/>
-      <c r="I47" s="8"/>
-    </row>
-    <row r="48" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-    </row>
-    <row r="49" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-    </row>
-    <row r="50" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A50" s="8"/>
-      <c r="B50" s="8"/>
-    </row>
-    <row r="51" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A51" s="8"/>
-      <c r="B51" s="8"/>
-    </row>
-    <row r="52" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A52" s="8"/>
-      <c r="B52" s="8"/>
-    </row>
-    <row r="53" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A53" s="8"/>
-      <c r="B53" s="8"/>
-    </row>
-    <row r="54" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A54" s="8"/>
-      <c r="B54" s="8"/>
-    </row>
-    <row r="55" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="8"/>
-    </row>
-    <row r="56" spans="1:2" ht="23.25" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="8"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="11"/>
+      <c r="B47" s="11"/>
+      <c r="C47" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D47" s="11"/>
+      <c r="E47" s="11"/>
+      <c r="F47" s="11"/>
+      <c r="G47" s="11"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="11"/>
+    </row>
+    <row r="48" spans="1:12" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="11"/>
+      <c r="B48" s="11"/>
+    </row>
+    <row r="49" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="11"/>
+      <c r="B49" s="11"/>
+    </row>
+    <row r="50" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="11"/>
+      <c r="B50" s="11"/>
+    </row>
+    <row r="51" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="11"/>
+      <c r="B51" s="11"/>
+    </row>
+    <row r="52" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="11"/>
+      <c r="B52" s="11"/>
+    </row>
+    <row r="53" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="11"/>
+      <c r="B53" s="11"/>
+    </row>
+    <row r="54" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="11"/>
+      <c r="B54" s="11"/>
+    </row>
+    <row r="55" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="11"/>
+      <c r="B55" s="11"/>
+    </row>
+    <row r="56" spans="1:2" ht="23.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="11"/>
+      <c r="B56" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="C43:I43"/>
-    <mergeCell ref="A27:B28"/>
-    <mergeCell ref="A30:B31"/>
-    <mergeCell ref="A33:B34"/>
+    <mergeCell ref="A47:B47"/>
+    <mergeCell ref="A32:B32"/>
     <mergeCell ref="A37:B38"/>
     <mergeCell ref="A41:B42"/>
     <mergeCell ref="A45:B46"/>
     <mergeCell ref="C35:J35"/>
     <mergeCell ref="C39:I39"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="C17:J17"/>
-    <mergeCell ref="A15:B16"/>
-    <mergeCell ref="A5:B6"/>
-    <mergeCell ref="A8:B9"/>
-    <mergeCell ref="A11:B12"/>
-    <mergeCell ref="F11:I11"/>
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A55:B55"/>
     <mergeCell ref="A56:B56"/>
@@ -1581,28 +1609,38 @@
     <mergeCell ref="A51:B51"/>
     <mergeCell ref="A52:B52"/>
     <mergeCell ref="A53:B53"/>
-    <mergeCell ref="A47:B47"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="F45:I45"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
     <mergeCell ref="A23:B23"/>
     <mergeCell ref="A2:B2"/>
-    <mergeCell ref="F37:I37"/>
     <mergeCell ref="F5:I5"/>
     <mergeCell ref="F8:I8"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="F33:I33"/>
-    <mergeCell ref="F27:I27"/>
     <mergeCell ref="F20:I20"/>
-    <mergeCell ref="F30:I30"/>
-    <mergeCell ref="A32:B32"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="C17:J17"/>
+    <mergeCell ref="A15:B16"/>
+    <mergeCell ref="A5:B6"/>
+    <mergeCell ref="A8:B9"/>
+    <mergeCell ref="A11:B12"/>
+    <mergeCell ref="F11:I11"/>
     <mergeCell ref="F24:I24"/>
     <mergeCell ref="C22:K22"/>
     <mergeCell ref="A20:B21"/>
     <mergeCell ref="A24:B25"/>
+    <mergeCell ref="A48:B48"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="F45:I45"/>
+    <mergeCell ref="F37:I37"/>
+    <mergeCell ref="F33:I33"/>
+    <mergeCell ref="F27:I27"/>
+    <mergeCell ref="F30:I30"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="C43:I43"/>
+    <mergeCell ref="A27:B28"/>
+    <mergeCell ref="A30:B31"/>
+    <mergeCell ref="A33:B34"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1611,12 +1649,12 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1625,12 +1663,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>